<commit_message>
Updated Backend to use AirTable
</commit_message>
<xml_diff>
--- a/contact_data.xlsx
+++ b/contact_data.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="18">
   <si>
     <t>Name</t>
   </si>
@@ -62,6 +62,9 @@
   </si>
   <si>
     <t>3/13/2025, 1:25:33 PM</t>
+  </si>
+  <si>
+    <t>3/13/2025, 4:18:19 PM</t>
   </si>
 </sst>
 </file>
@@ -438,7 +441,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D6"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -509,6 +512,20 @@
       </c>
       <c r="D5" t="s">
         <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>